<commit_message>
Remove RSDAHT2 (use RSDAHT instead)
</commit_message>
<xml_diff>
--- a/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
+++ b/SuppXLS/Scen_B_SYS_MaxGrowthRates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Olex\Documents\MANRID\ResLab\Modelling\TIMES\TIMES-IE\SuppXLS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TIMES-models\TIM\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{079ABAE7-500A-4B66-BADB-A105DB66B61A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681A9071-3F44-4AF1-AAAA-93C474775303}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
+    <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{39DC52AD-7AD8-48BE-9D85-AA1C40791A2D}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="6" r:id="rId1"/>
@@ -22,9 +22,6 @@
     <sheet name="RSD-Retrofits" sheetId="9" r:id="rId7"/>
     <sheet name="TRA" sheetId="1" r:id="rId8"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId9"/>
-  </externalReferences>
   <definedNames>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="0" hidden="1">#REF!</definedName>
     <definedName name="__123Graph_AEUMILKPN" localSheetId="3" hidden="1">#REF!</definedName>
@@ -870,9 +867,6 @@
     <t>SRVAHT,SRVAHT2</t>
   </si>
   <si>
-    <t>RSDAHT,RSDAHT2</t>
-  </si>
-  <si>
     <t>BIOGAS1G,BIOGAS2G</t>
   </si>
   <si>
@@ -907,6 +901,9 @@
   </si>
   <si>
     <t>SBIORETH*</t>
+  </si>
+  <si>
+    <t>RSDAHT</t>
   </si>
 </sst>
 </file>
@@ -1290,6 +1287,7 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="4" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1302,7 +1300,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1700,33 +1697,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Cover"/>
-      <sheetName val="Regions"/>
-      <sheetName val="SUP"/>
-      <sheetName val="PWR"/>
-      <sheetName val="RSD"/>
-      <sheetName val="RSD-Retrofits"/>
-      <sheetName val="SRV"/>
-      <sheetName val="TRA"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2465,12 +2435,12 @@
       <c r="Z15" s="31"/>
     </row>
     <row r="16" spans="1:26" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="51" t="s">
+      <c r="A16" s="52" t="s">
         <v>161</v>
       </c>
-      <c r="B16" s="51"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="51"/>
+      <c r="B16" s="52"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="52"/>
       <c r="E16" s="32"/>
       <c r="F16" s="32"/>
       <c r="G16" s="33"/>
@@ -2554,11 +2524,11 @@
       <c r="A19" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="B19" s="50" t="s">
+      <c r="B19" s="51" t="s">
         <v>173</v>
       </c>
-      <c r="C19" s="50"/>
-      <c r="D19" s="50"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="51"/>
       <c r="E19" s="38"/>
       <c r="F19" s="38"/>
       <c r="G19" s="39"/>
@@ -2586,11 +2556,11 @@
       <c r="A20" s="37" t="s">
         <v>163</v>
       </c>
-      <c r="B20" s="50" t="s">
+      <c r="B20" s="51" t="s">
         <v>176</v>
       </c>
-      <c r="C20" s="50"/>
-      <c r="D20" s="50"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="51"/>
       <c r="E20" s="38"/>
       <c r="F20" s="38"/>
       <c r="G20" s="39"/>
@@ -2678,11 +2648,11 @@
       <c r="A23" s="37" t="s">
         <v>165</v>
       </c>
-      <c r="B23" s="50" t="s">
+      <c r="B23" s="51" t="s">
         <v>178</v>
       </c>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="51"/>
       <c r="E23" s="31"/>
       <c r="F23" s="31"/>
       <c r="G23" s="31"/>
@@ -2708,11 +2678,11 @@
     </row>
     <row r="24" spans="1:26" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="37"/>
-      <c r="B24" s="50" t="s">
+      <c r="B24" s="51" t="s">
         <v>174</v>
       </c>
-      <c r="C24" s="50"/>
-      <c r="D24" s="50"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="51"/>
       <c r="E24" s="31"/>
       <c r="F24" s="31"/>
       <c r="G24" s="31"/>
@@ -2770,11 +2740,11 @@
       <c r="A26" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="B26" s="50" t="s">
+      <c r="B26" s="51" t="s">
         <v>175</v>
       </c>
-      <c r="C26" s="50"/>
-      <c r="D26" s="50"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="51"/>
       <c r="E26" s="31"/>
       <c r="F26" s="31"/>
       <c r="G26" s="31"/>
@@ -2890,11 +2860,11 @@
       <c r="A30" s="37" t="s">
         <v>168</v>
       </c>
-      <c r="B30" s="52" t="s">
+      <c r="B30" s="53" t="s">
         <v>169</v>
       </c>
-      <c r="C30" s="50"/>
-      <c r="D30" s="50"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="51"/>
       <c r="E30" s="42"/>
       <c r="F30" s="42"/>
       <c r="G30" s="31"/>
@@ -2922,11 +2892,11 @@
       <c r="A31" s="37" t="s">
         <v>170</v>
       </c>
-      <c r="B31" s="50" t="s">
+      <c r="B31" s="51" t="s">
         <v>171</v>
       </c>
-      <c r="C31" s="50"/>
-      <c r="D31" s="50"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="51"/>
       <c r="E31" s="42"/>
       <c r="F31" s="42"/>
       <c r="G31" s="31"/>
@@ -5646,7 +5616,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89417C8F-9D07-4311-9372-0B0C534E50C4}">
   <dimension ref="A2:N19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
@@ -5786,7 +5756,7 @@
         <v>144</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E7" s="2">
         <v>2018</v>
@@ -5822,7 +5792,7 @@
         <v>144</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="E8" s="2">
         <v>2018</v>
@@ -5888,7 +5858,7 @@
         <v>186</v>
       </c>
       <c r="B13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C13" s="11">
         <v>0.4</v>
@@ -5902,7 +5872,7 @@
         <v>186</v>
       </c>
       <c r="B14" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C14" s="11">
         <v>0.4</v>
@@ -5962,7 +5932,7 @@
         <v>2222</v>
       </c>
       <c r="H19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -6520,8 +6490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9933FEB4-63EA-406B-A848-C3344FC12632}">
   <dimension ref="A2:N37"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6642,7 +6612,7 @@
       </c>
       <c r="D6" s="2"/>
       <c r="F6" s="2" t="s">
-        <v>221</v>
+        <v>233</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>142</v>
@@ -7348,7 +7318,7 @@
       </c>
       <c r="H37" t="str">
         <f xml:space="preserve"> _xlfn.TEXTJOIN(",",TRUE,F6:F17)</f>
-        <v>RSDAHT,RSDAHT2,RSDBDL,RSDWOO,RSDCOA,RSDPEA,RSDELC,RSDETH,RSDGAS,RSDHET,RSDLPG,RSDKER,RSDSOL</v>
+        <v>RSDAHT,RSDBDL,RSDWOO,RSDCOA,RSDPEA,RSDELC,RSDETH,RSDGAS,RSDHET,RSDLPG,RSDKER,RSDSOL</v>
       </c>
     </row>
   </sheetData>
@@ -7925,7 +7895,7 @@
         <v>181</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="L5" s="4" t="s">
         <v>182</v>
@@ -7943,12 +7913,12 @@
         <v>UC_RSD_MaxGrowth_Retrofits</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H6" s="2">
         <v>2019</v>
@@ -7977,13 +7947,13 @@
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="H7">
         <v>2019</v>
@@ -7991,7 +7961,7 @@
       <c r="I7" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="J7" s="54">
+      <c r="J7" s="50">
         <v>1</v>
       </c>
       <c r="K7" s="2"/>
@@ -8002,7 +7972,7 @@
         <v>5</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -8010,7 +7980,7 @@
         <v>117</v>
       </c>
       <c r="D9" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -8018,7 +7988,7 @@
         <v>195</v>
       </c>
       <c r="B10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C10" s="11">
         <v>0.5</v>
@@ -8966,7 +8936,7 @@
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A30" s="53" t="s">
+      <c r="A30" s="54" t="s">
         <v>27</v>
       </c>
       <c r="B30" t="s">
@@ -8996,7 +8966,7 @@
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A31" s="53"/>
+      <c r="A31" s="54"/>
       <c r="B31" t="s">
         <v>25</v>
       </c>
@@ -9024,7 +8994,7 @@
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A32" s="53"/>
+      <c r="A32" s="54"/>
       <c r="B32" t="s">
         <v>24</v>
       </c>
@@ -9052,7 +9022,7 @@
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A33" s="53"/>
+      <c r="A33" s="54"/>
       <c r="B33" t="s">
         <v>23</v>
       </c>
@@ -9080,7 +9050,7 @@
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A34" s="53"/>
+      <c r="A34" s="54"/>
       <c r="B34" t="s">
         <v>22</v>
       </c>
@@ -9108,7 +9078,7 @@
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A35" s="53"/>
+      <c r="A35" s="54"/>
       <c r="B35" t="s">
         <v>21</v>
       </c>
@@ -9697,9 +9667,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9914,19 +9887,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -9951,9 +9920,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{62402F5C-4915-4658-8F60-3A11655231DF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BB3709B4-63F5-4DFC-B992-07B9DE433FAB}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>